<commit_message>
데이터 상 CC 완료 + Turtle Passive 구현 완료
- Turtle의 이동 처리는 아직 미구현(기획 사항 없음)
</commit_message>
<xml_diff>
--- a/DataGenerator/XLSXS/CharData.xlsx
+++ b/DataGenerator/XLSXS/CharData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunja\Documents\DG_Project\DataGenerator\XLSXS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jehee\Documents\GitHub\DG_Project\DataGenerator\XLSXS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A416FC3-406C-4391-864B-C0644181FE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE58E69-94D0-4590-B76E-FEC8EBDCDE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="154">
   <si>
     <t>charID</t>
   </si>
@@ -479,6 +479,10 @@
   </si>
   <si>
     <t>MECHA:TIDY3_Enemy_Prefab</t>
+  </si>
+  <si>
+    <t>[501710]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -811,8 +815,8 @@
   </sheetPr>
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1666,11 +1670,9 @@
         <v>52</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="3">
-        <v>501700</v>
-      </c>
+      <c r="J22" s="3"/>
       <c r="K22" s="3" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>145</v>
@@ -2498,7 +2500,7 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>145</v>

</xml_diff>